<commit_message>
Fix typo, changed `insetRows` into `insertRows`. The old version should be removed further. Fixed fixture file- replaced `__interated` by `__last` closes https://github.com/Siemienik/XToolset/issues/96
</commit_message>
<xml_diff>
--- a/packages/xlsx-renderer/tests/integration/data/Renderer012-ForEach-special/template.xlsx
+++ b/packages/xlsx-renderer/tests/integration/data/Renderer012-ForEach-special/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siemi\aProjects\xlsx-renderer-2\tests\integration\data\Renderer012-ForEach-special\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemienik/WebstormProjects/xlsx-import/packages/xlsx-renderer/tests/integration/data/Renderer012-ForEach-special/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0771BF14-1C2C-4AFF-A18F-F44B05B240EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD59F583-5582-2E45-9B31-315B04CFFAE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27795" windowHeight="16440" activeTab="2" xr2:uid="{51D64FAE-FDF3-4046-A668-3472FA61F864}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27800" windowHeight="16440" xr2:uid="{51D64FAE-FDF3-4046-A668-3472FA61F864}"/>
   </bookViews>
   <sheets>
     <sheet name="Most common for each" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="78">
   <si>
     <t>FOR EACH special item</t>
   </si>
@@ -251,7 +251,22 @@
     <t>#! WS_NAME name</t>
   </si>
   <si>
-    <t>#! FINISH item.__iterated</t>
+    <t>__last</t>
+  </si>
+  <si>
+    <t>`__last` - is this last element of a collection</t>
+  </si>
+  <si>
+    <t>## item.__last</t>
+  </si>
+  <si>
+    <t>&lt;- delete item</t>
+  </si>
+  <si>
+    <t>#! FINISH item.__last</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> item.__last</t>
   </si>
 </sst>
 </file>
@@ -661,20 +676,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CB5A86-9F62-4CA9-8E69-0560B4CC82E1}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="10" customWidth="1"/>
-    <col min="11" max="16" width="13.5703125" customWidth="1"/>
-    <col min="17" max="18" width="10" customWidth="1"/>
+    <col min="1" max="11" width="10" customWidth="1"/>
+    <col min="12" max="17" width="13.5" customWidth="1"/>
+    <col min="18" max="19" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,328 +708,342 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="Q1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1"/>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="1"/>
+      <c r="O2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q2" s="1"/>
+      <c r="R2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>17</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>19</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>20</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>21</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>32</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>33</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>34</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>35</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>36</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>37</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>38</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="Q6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>29</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>31</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>32</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>33</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>34</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>35</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>36</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>37</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>38</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>39</v>
       </c>
-      <c r="Q7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="E11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>43</v>
       </c>
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
-      <c r="E13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="E14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="F17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="E17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>50</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1022,325 +1051,343 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA1F4E2-D67A-408E-882F-920444C906FB}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16" width="16.5703125" customWidth="1"/>
+    <col min="1" max="17" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>32</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>34</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>35</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>37</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>38</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
       <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>31</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>32</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>33</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>34</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>35</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>36</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>37</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>38</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>13</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>14</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>15</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>16</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>17</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>18</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>19</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>20</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>21</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>22</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>29</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>31</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>32</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>33</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>34</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>35</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>36</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>37</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>38</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>39</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1351,18 +1398,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209109B6-BA88-4AF5-9D3F-FCC154609ECE}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="28.42578125" customWidth="1"/>
+    <col min="1" max="3" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1373,7 +1420,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1384,207 +1431,218 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>56</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>57</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>58</v>
       </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>59</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>60</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>61</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>62</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>63</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>64</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="C11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>65</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>66</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>67</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>68</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>37</v>
       </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>69</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>70</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>71</v>
       </c>
-      <c r="C23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>72</v>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>